<commit_message>
Add Few More TestCases And Refactor Structure
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/AdvancedTestsData/DragAndDropData.xlsx
+++ b/src/test/java/TestData/AdvancedTestsData/DragAndDropData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateusz\SeleniumEasyFramework_Project\src\test\java\TestData\AdvancedTestsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA6D229-1D92-4DB0-8936-837C9E3D1C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4EE491-AA00-4ACD-813B-69E29CAF7219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21645" windowHeight="11385" activeTab="1" xr2:uid="{9A86680D-3610-44A9-A6BF-82B3857DD803}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21645" windowHeight="11385" activeTab="1" xr2:uid="{9A86680D-3610-44A9-A6BF-82B3857DD803}"/>
   </bookViews>
   <sheets>
     <sheet name="dragAndDropDragItemData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>value</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>expected</t>
-  </si>
-  <si>
-    <t>expected2</t>
-  </si>
-  <si>
-    <t>expected1</t>
   </si>
 </sst>
 </file>
@@ -420,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8264AE5E-F596-4F13-842A-B93D27C58748}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,44 +425,29 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -479,28 +458,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16B2209-958F-4A11-912D-5922691DB2BE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
         <v>4</v>
       </c>
     </row>

</xml_diff>